<commit_message>
Good fit of all sites with basal area and new vernalisation model.
</commit_message>
<xml_diff>
--- a/model/WCST Notes.xlsx
+++ b/model/WCST Notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="6180" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>(OC)</t>
   </si>
@@ -65,9 +65,6 @@
     <t>triplicate</t>
   </si>
   <si>
-    <t>measurements.</t>
-  </si>
-  <si>
     <t>Horizon</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>BD</t>
   </si>
   <si>
-    <t>DC</t>
-  </si>
-  <si>
     <t>FC</t>
   </si>
   <si>
@@ -158,21 +152,12 @@
     <t>cultivated)</t>
   </si>
   <si>
-    <t>27.S</t>
-  </si>
-  <si>
     <t>(O.OS)</t>
   </si>
   <si>
-    <t>26.S</t>
-  </si>
-  <si>
     <t>(O.S)</t>
   </si>
   <si>
-    <t>3S.0</t>
-  </si>
-  <si>
     <t>(short-term</t>
   </si>
   <si>
@@ -209,9 +194,6 @@
     <t>35-40</t>
   </si>
   <si>
-    <t>S1.3</t>
-  </si>
-  <si>
     <t>55-60</t>
   </si>
   <si>
@@ -255,6 +237,33 @@
   </si>
   <si>
     <t>Table from Grewal et al 1990 (OCR so some mistakes)</t>
+  </si>
+  <si>
+    <t>WCST</t>
+  </si>
+  <si>
+    <t>WCFC</t>
+  </si>
+  <si>
+    <t>FWCFC</t>
+  </si>
+  <si>
+    <t>WCWP</t>
+  </si>
+  <si>
+    <t>FWCWP</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>OC</t>
   </si>
 </sst>
 </file>
@@ -615,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P50"/>
+  <dimension ref="B1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,12 +635,68 @@
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1">
+        <f>MIN(E7:E45)</f>
+        <v>0.83</v>
+      </c>
+      <c r="P1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q1">
+        <f>MIN(Q7:Q45)</f>
+        <v>44.08</v>
+      </c>
+      <c r="R1">
+        <f>MIN(R7:R45)</f>
+        <v>31.46</v>
+      </c>
+      <c r="S1">
+        <f>MIN(S7:S45)</f>
+        <v>0.55597014925373134</v>
+      </c>
+      <c r="T1">
+        <f>MIN(T7:T45)</f>
+        <v>13.92</v>
+      </c>
+      <c r="U1">
+        <f>MIN(U7:U45)</f>
+        <v>0.31210191082802546</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>AVERAGE(E7:E45)</f>
+        <v>1.2384615384615383</v>
+      </c>
+      <c r="P2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2">
+        <f>AVERAGE(Q7:Q45)</f>
+        <v>60.832974358974347</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2:U2" si="0">AVERAGE(R7:R45)</f>
+        <v>39.311051282051288</v>
+      </c>
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>0.65146111324495304</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>26.201435897435896</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>0.42200191192694392</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -641,8 +706,9 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>3</v>
+      <c r="E3">
+        <f>MAX(E7:E45)</f>
+        <v>1.58</v>
       </c>
       <c r="F3" t="s">
         <v>4</v>
@@ -675,81 +741,113 @@
         <v>12</v>
       </c>
       <c r="P3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q3">
+        <f>MAX(Q7:Q45)</f>
+        <v>100.92599999999999</v>
+      </c>
+      <c r="R3">
+        <f>MAX(R7:R45)</f>
+        <v>57.204000000000001</v>
+      </c>
+      <c r="S3">
+        <f>MAX(S7:S45)</f>
+        <v>0.7449275362318839</v>
+      </c>
+      <c r="T3">
+        <f>MAX(T7:T45)</f>
+        <v>46.32</v>
+      </c>
+      <c r="U3">
+        <f>MAX(U7:U45)</f>
+        <v>0.58528951486697967</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>21</v>
       </c>
-      <c r="L5" t="s">
+      <c r="Q5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" t="s">
+        <v>73</v>
+      </c>
+      <c r="T5" t="s">
+        <v>74</v>
+      </c>
+      <c r="U5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="N5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="3">
         <v>1.28</v>
@@ -784,14 +882,34 @@
       <c r="O7">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <f>N7*E7</f>
+        <v>57.728000000000002</v>
+      </c>
+      <c r="R7">
+        <f>H7*E7</f>
+        <v>40.576000000000001</v>
+      </c>
+      <c r="S7">
+        <f>R7/Q7</f>
+        <v>0.70288248337028825</v>
+      </c>
+      <c r="T7">
+        <f>J7*E7</f>
+        <v>31.231999999999999</v>
+      </c>
+      <c r="U7">
+        <f>T7/Q7</f>
+        <v>0.54101995565410199</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1">
         <v>43378</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3">
         <v>1.27</v>
@@ -826,14 +944,34 @@
       <c r="O8">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q45" si="1">N8*E8</f>
+        <v>53.594000000000001</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8:R45" si="2">H8*E8</f>
+        <v>39.116</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ref="S8:S45" si="3">R8/Q8</f>
+        <v>0.72985781990521326</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T45" si="4">J8*E8</f>
+        <v>27.812999999999999</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ref="U8:U45" si="5">T8/Q8</f>
+        <v>0.51895734597156395</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2">
         <v>42278</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3">
         <v>1.21</v>
@@ -868,13 +1006,33 @@
       <c r="O9">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>55.055</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>39.93</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="3"/>
+        <v>0.72527472527472525</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>28.677</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="5"/>
+        <v>0.52087912087912092</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3">
         <v>1.1499999999999999</v>
@@ -909,13 +1067,33 @@
       <c r="O10">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>45.54</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>32.084999999999994</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="3"/>
+        <v>0.70454545454545447</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="4"/>
+        <v>21.849999999999998</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="5"/>
+        <v>0.47979797979797978</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3">
         <v>1.35</v>
@@ -950,16 +1128,36 @@
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>32.67</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="3"/>
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="4"/>
+        <v>22.410000000000004</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="5"/>
+        <v>0.41500000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2">
         <v>42064</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E12" s="3">
         <v>1.22</v>
@@ -994,13 +1192,33 @@
       <c r="O12">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>56.73</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>38.917999999999999</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="3"/>
+        <v>0.6860215053763441</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="4"/>
+        <v>26.474</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="5"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E13" s="3">
         <v>1.58</v>
@@ -1035,13 +1253,33 @@
       <c r="O13">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>51.981999999999999</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>31.6</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="3"/>
+        <v>0.60790273556231011</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="4"/>
+        <v>18.170000000000002</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="5"/>
+        <v>0.34954407294832829</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E14" s="3">
         <v>1.3</v>
@@ -1076,13 +1314,33 @@
       <c r="O14">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <f t="shared" si="1"/>
+        <v>60.97</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="2"/>
+        <v>35.1</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="3"/>
+        <v>0.57569296375266532</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="4"/>
+        <v>20.150000000000002</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="5"/>
+        <v>0.33049040511727085</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3">
         <v>1.5</v>
@@ -1117,16 +1375,36 @@
       <c r="O15">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <f t="shared" si="1"/>
+        <v>62.550000000000004</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="2"/>
+        <v>41.400000000000006</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="3"/>
+        <v>0.66187050359712229</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="4"/>
+        <v>24.299999999999997</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="5"/>
+        <v>0.38848920863309344</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3">
         <v>1.17</v>
@@ -1161,16 +1439,36 @@
       <c r="O16">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <f t="shared" si="1"/>
+        <v>57.33</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="2"/>
+        <v>38.259</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="3"/>
+        <v>0.66734693877551021</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="4"/>
+        <v>24.335999999999999</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="5"/>
+        <v>0.42448979591836733</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1">
         <v>43378</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E17" s="3">
         <v>1.28</v>
@@ -1205,16 +1503,36 @@
       <c r="O17">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <f t="shared" si="1"/>
+        <v>55.936000000000007</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="2"/>
+        <v>35.328000000000003</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="3"/>
+        <v>0.63157894736842102</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="4"/>
+        <v>21.888000000000002</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="5"/>
+        <v>0.39130434782608692</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2">
         <v>42278</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3">
         <v>1.21</v>
@@ -1249,13 +1567,33 @@
       <c r="O18">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <f t="shared" si="1"/>
+        <v>49.852000000000004</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="2"/>
+        <v>32.186</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="3"/>
+        <v>0.64563106796116498</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="4"/>
+        <v>20.57</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="5"/>
+        <v>0.41262135922330095</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3">
         <v>1.27</v>
@@ -1290,13 +1628,33 @@
       <c r="O19">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <f t="shared" si="1"/>
+        <v>52.577999999999996</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="2"/>
+        <v>32.512</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="3"/>
+        <v>0.6183574879227054</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="4"/>
+        <v>20.701000000000001</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="5"/>
+        <v>0.39371980676328505</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3">
         <v>1.3</v>
@@ -1331,16 +1689,36 @@
       <c r="O20">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <f t="shared" si="1"/>
+        <v>52.260000000000005</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="2"/>
+        <v>32.5</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="3"/>
+        <v>0.62189054726368154</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="4"/>
+        <v>20.28</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="5"/>
+        <v>0.38805970149253732</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
         <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
       </c>
       <c r="E21" s="3">
         <v>1.27</v>
@@ -1375,16 +1753,36 @@
       <c r="O21">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <f t="shared" si="1"/>
+        <v>59.817</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="2"/>
+        <v>36.322000000000003</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="3"/>
+        <v>0.60721868365180476</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="4"/>
+        <v>18.669</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="5"/>
+        <v>0.31210191082802546</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1">
         <v>43378</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3">
         <v>1.21</v>
@@ -1419,16 +1817,36 @@
       <c r="O22">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <f t="shared" si="1"/>
+        <v>56.991</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="2"/>
+        <v>33.879999999999995</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="3"/>
+        <v>0.59447983014861994</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="4"/>
+        <v>18.513000000000002</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="5"/>
+        <v>0.32484076433121023</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="2">
         <v>42278</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" s="3">
         <v>1.1499999999999999</v>
@@ -1463,13 +1881,33 @@
       <c r="O23">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <f t="shared" si="1"/>
+        <v>52.669999999999995</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="2"/>
+        <v>33.234999999999992</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="3"/>
+        <v>0.63100436681222705</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="4"/>
+        <v>16.904999999999998</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="5"/>
+        <v>0.3209606986899563</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3">
         <v>1.19</v>
@@ -1480,8 +1918,8 @@
       <c r="G24">
         <v>2.59</v>
       </c>
-      <c r="H24" t="s">
-        <v>44</v>
+      <c r="H24">
+        <v>27.5</v>
       </c>
       <c r="I24">
         <v>-0.5</v>
@@ -1504,19 +1942,39 @@
       <c r="O24">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>52.240999999999993</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="2"/>
+        <v>32.725000000000001</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="3"/>
+        <v>0.62642369020501154</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="4"/>
+        <v>16.66</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="5"/>
+        <v>0.31890660592255132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E25" s="3">
         <v>1.51</v>
       </c>
       <c r="F25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G25">
         <v>0.75</v>
@@ -1545,16 +2003,36 @@
       <c r="O25">
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <f t="shared" si="1"/>
+        <v>44.998000000000005</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="2"/>
+        <v>31.71</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="3"/>
+        <v>0.70469798657718119</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="4"/>
+        <v>16.157</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="5"/>
+        <v>0.35906040268456374</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
         <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
       </c>
       <c r="E26" s="3">
         <v>1.33</v>
@@ -1565,8 +2043,8 @@
       <c r="G26">
         <v>2.4700000000000002</v>
       </c>
-      <c r="H26" t="s">
-        <v>46</v>
+      <c r="H26">
+        <v>26.5</v>
       </c>
       <c r="I26">
         <v>-0.5</v>
@@ -1575,7 +2053,7 @@
         <v>13.1</v>
       </c>
       <c r="K26" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L26">
         <v>13.6</v>
@@ -1583,22 +2061,42 @@
       <c r="M26">
         <v>-1</v>
       </c>
-      <c r="N26" t="s">
-        <v>48</v>
+      <c r="N26">
+        <v>38</v>
       </c>
       <c r="O26">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <f t="shared" si="1"/>
+        <v>50.540000000000006</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="2"/>
+        <v>35.245000000000005</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="3"/>
+        <v>0.69736842105263164</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="4"/>
+        <v>17.423000000000002</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="5"/>
+        <v>0.34473684210526317</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1">
         <v>43378</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E27" s="3">
         <v>1.37</v>
@@ -1633,16 +2131,36 @@
       <c r="O27">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <f t="shared" si="1"/>
+        <v>54.115000000000002</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="2"/>
+        <v>38.634</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="3"/>
+        <v>0.71392405063291142</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="4"/>
+        <v>19.18</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="5"/>
+        <v>0.35443037974683544</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2">
         <v>42278</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E28" s="3">
         <v>1.41</v>
@@ -1677,13 +2195,33 @@
       <c r="O28">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <f t="shared" si="1"/>
+        <v>53.297999999999995</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="2"/>
+        <v>36.095999999999997</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="3"/>
+        <v>0.67724867724867721</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="4"/>
+        <v>17.201999999999998</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="5"/>
+        <v>0.32275132275132273</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E29" s="3">
         <v>1.38</v>
@@ -1718,13 +2256,33 @@
       <c r="O29">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <f t="shared" si="1"/>
+        <v>47.61</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="2"/>
+        <v>35.465999999999994</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="3"/>
+        <v>0.7449275362318839</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="4"/>
+        <v>16.974</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="5"/>
+        <v>0.35652173913043478</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3">
         <v>1.45</v>
@@ -1759,16 +2317,36 @@
       <c r="O30">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>44.08</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="2"/>
+        <v>32.625</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="3"/>
+        <v>0.74013157894736847</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="4"/>
+        <v>13.92</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="5"/>
+        <v>0.31578947368421056</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E31" s="3">
         <v>1.1499999999999999</v>
@@ -1803,16 +2381,36 @@
       <c r="O31">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>63.709999999999994</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="2"/>
+        <v>38.64</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="3"/>
+        <v>0.60649819494584845</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="4"/>
+        <v>24.494999999999997</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="5"/>
+        <v>0.3844765342960289</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1">
         <v>43378</v>
       </c>
       <c r="D32" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E32" s="3">
         <v>1.21</v>
@@ -1847,16 +2445,36 @@
       <c r="O32">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>58.564</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="2"/>
+        <v>37.994</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="3"/>
+        <v>0.64876033057851235</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="4"/>
+        <v>22.868999999999996</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="5"/>
+        <v>0.39049586776859496</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C33" s="2">
         <v>42278</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E33" s="3">
         <v>1.31</v>
@@ -1891,19 +2509,39 @@
       <c r="O33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>54.365000000000002</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="2"/>
+        <v>34.06</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="3"/>
+        <v>0.62650602409638556</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="4"/>
+        <v>22.401000000000003</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="5"/>
+        <v>0.4120481927710844</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E34" s="3">
         <v>1.3</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G34">
         <v>2.57</v>
@@ -1932,13 +2570,33 @@
       <c r="O34">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>51.87</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="2"/>
+        <v>31.46</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="3"/>
+        <v>0.60651629072681712</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="4"/>
+        <v>21.19</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="5"/>
+        <v>0.4085213032581454</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E35" s="3">
         <v>1.37</v>
@@ -1973,22 +2631,42 @@
       <c r="O35">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <f t="shared" si="1"/>
+        <v>49.868000000000002</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="2"/>
+        <v>31.921000000000003</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="3"/>
+        <v>0.64010989010989017</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="4"/>
+        <v>21.509</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="5"/>
+        <v>0.43131868131868129</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1">
         <v>43378</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E36" s="3">
         <v>0.83</v>
       </c>
       <c r="F36" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G36">
         <v>6.33</v>
@@ -2017,19 +2695,39 @@
       <c r="O36">
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <f t="shared" si="1"/>
+        <v>74.119</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="2"/>
+        <v>47.641999999999996</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>0.64277715565509508</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="4"/>
+        <v>33.366</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="5"/>
+        <v>0.45016797312430012</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E37" s="3">
         <v>0.9</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G37">
         <v>3.12</v>
@@ -2058,19 +2756,39 @@
       <c r="O37">
         <v>-1.1000000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <f t="shared" si="1"/>
+        <v>68.58</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="2"/>
+        <v>47.7</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>0.69553805774278221</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="4"/>
+        <v>35.369999999999997</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="5"/>
+        <v>0.51574803149606296</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E38" s="3">
         <v>1.02</v>
       </c>
       <c r="F38" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G38">
         <v>1.61</v>
@@ -2093,19 +2811,39 @@
       <c r="M38">
         <v>-0.8</v>
       </c>
-      <c r="N38" t="s">
-        <v>61</v>
+      <c r="N38">
+        <v>81.3</v>
       </c>
       <c r="O38">
         <v>-0.9</v>
       </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <f t="shared" si="1"/>
+        <v>82.926000000000002</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="2"/>
+        <v>54.161999999999999</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>0.65313653136531358</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="4"/>
+        <v>42.432000000000002</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="5"/>
+        <v>0.51168511685116858</v>
+      </c>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -2140,13 +2878,33 @@
       <c r="O39">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>84.1</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="2"/>
+        <v>53.8</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="3"/>
+        <v>0.63971462544589774</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="4"/>
+        <v>41.8</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="5"/>
+        <v>0.49702734839476814</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E40" s="3">
         <v>1.03</v>
@@ -2181,16 +2939,36 @@
       <c r="O40">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>80.031000000000006</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="2"/>
+        <v>53.045000000000002</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="3"/>
+        <v>0.66280566280566278</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="4"/>
+        <v>42.024000000000001</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="5"/>
+        <v>0.52509652509652505</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C41" s="1">
         <v>43378</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E41" s="3">
         <v>1.07</v>
@@ -2225,14 +3003,34 @@
       <c r="O41">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <f t="shared" si="1"/>
+        <v>67.624000000000009</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="2"/>
+        <v>46.010000000000005</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="3"/>
+        <v>0.680379746835443</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="4"/>
+        <v>39.055</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="5"/>
+        <v>0.57753164556962022</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2">
         <v>43070</v>
       </c>
       <c r="D42" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E42" s="3">
         <v>1.08</v>
@@ -2267,13 +3065,33 @@
       <c r="O42">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <f t="shared" si="1"/>
+        <v>69.012</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="2"/>
+        <v>47.52</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="3"/>
+        <v>0.68857589984350553</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="4"/>
+        <v>40.392000000000003</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="5"/>
+        <v>0.58528951486697967</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E43" s="3">
         <v>1.21</v>
@@ -2308,13 +3126,33 @@
       <c r="O43">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <f t="shared" si="1"/>
+        <v>87.845999999999989</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="2"/>
+        <v>50.214999999999996</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="3"/>
+        <v>0.57162534435261714</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="4"/>
+        <v>43.197000000000003</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="5"/>
+        <v>0.49173553719008273</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E44" s="3">
         <v>1.2</v>
@@ -2349,13 +3187,33 @@
       <c r="O44">
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <f t="shared" si="1"/>
+        <v>96.48</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="2"/>
+        <v>53.64</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="3"/>
+        <v>0.55597014925373134</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="4"/>
+        <v>46.32</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="5"/>
+        <v>0.48009950248756217</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E45" s="3">
         <v>1.26</v>
@@ -2390,14 +3248,34 @@
       <c r="O45">
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <f t="shared" si="1"/>
+        <v>100.92599999999999</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="2"/>
+        <v>57.204000000000001</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="3"/>
+        <v>0.56679151061173538</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="4"/>
+        <v>44.982000000000006</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="5"/>
+        <v>0.44569288389513123</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E47">
         <f>AVERAGE(E7:E45)</f>
         <v>1.2384615384615383</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E48">
         <f>STDEV(E7:E45)</f>
         <v>0.1582060359075175</v>

</xml_diff>